<commit_message>
added prints and tests for missing schools in schools excel
</commit_message>
<xml_diff>
--- a/dashboard/apps/excel_import/excel_files/test_excels/b_test_db3.xlsx
+++ b/dashboard/apps/excel_import/excel_files/test_excels/b_test_db3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="52">
   <si>
     <t xml:space="preserve">Encrypted Student No</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t xml:space="preserve">00B197BA7753B1F2CFD57570245D62E8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00B197BA7753B1F2CFD57570245D62E9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASDF4242</t>
   </si>
 </sst>
 </file>
@@ -410,15 +416,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="16.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="17.2448979591837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,8 +1307,71 @@
         <v>33</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q15" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V15" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="45">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:K1"/>
@@ -1345,6 +1414,9 @@
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="I14:K14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixed for students who have empty final marks
</commit_message>
<xml_diff>
--- a/dashboard/apps/excel_import/excel_files/test_excels/b_test_db3.xlsx
+++ b/dashboard/apps/excel_import/excel_files/test_excels/b_test_db3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="53">
   <si>
     <t xml:space="preserve">Encrypted Student No</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">ASDF4242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00B197BA7753B1F2CFD57570245D6210</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
+      <selection pane="topLeft" activeCell="Q17" activeCellId="0" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="17.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,8 +1373,69 @@
         <v>33</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="48">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:K1"/>
@@ -1417,6 +1481,9 @@
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:K16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix for when the first instance of a student in a course doesn't have a mark
</commit_message>
<xml_diff>
--- a/dashboard/apps/excel_import/excel_files/test_excels/b_test_db3.xlsx
+++ b/dashboard/apps/excel_import/excel_files/test_excels/b_test_db3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="53">
   <si>
     <t xml:space="preserve">Encrypted Student No</t>
   </si>
@@ -419,15 +419,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q17" activeCellId="0" sqref="Q17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="20.4030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,8 +1409,8 @@
       <c r="O16" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>51</v>
+      <c r="P16" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="2" t="s">
@@ -1434,8 +1434,195 @@
         <v>33</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V17" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O18" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V18" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q19" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V19" s="3" t="n">
+        <v>63.67</v>
+      </c>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="57">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:K1"/>
@@ -1484,6 +1671,15 @@
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:K19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>